<commit_message>
Update benchmark results for .NET 7
</commit_message>
<xml_diff>
--- a/Docs/SdkPerformanceComparison.xlsx
+++ b/Docs/SdkPerformanceComparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\prometheus-net\prometheus-net\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\prometheus-net\prometheus-net\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15D1F04-4B17-4E64-A241-3726B17BC821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED97FE31-6C2A-49B1-8E66-96B9A1695C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22140" yWindow="1365" windowWidth="30030" windowHeight="18450" xr2:uid="{5D53A055-CCBA-4194-9E1E-2A7C459B8556}"/>
+    <workbookView xWindow="12690" yWindow="-16185" windowWidth="28770" windowHeight="15570" xr2:uid="{5D53A055-CCBA-4194-9E1E-2A7C459B8556}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>prometheus-net</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Setup</t>
   </si>
   <si>
-    <t>KiB</t>
-  </si>
-  <si>
     <t>Bytes</t>
   </si>
   <si>
@@ -77,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -120,7 +117,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -178,7 +175,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> bytes)</a:t>
+              <a:t> kilobytes)</a:t>
             </a:r>
             <a:endParaRPr lang="et-EE"/>
           </a:p>
@@ -260,7 +257,7 @@
                   <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3889472</c:v>
+                  <c:v>5919072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -311,7 +308,7 @@
                   <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7522320</c:v>
+                  <c:v>8682272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,7 +320,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -441,6 +437,9 @@
         <c:crossAx val="794333983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -647,10 +646,10 @@
                 <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>78.468000000000004</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1346.181</c:v>
+                  <c:v>1323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,10 +697,10 @@
                 <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>208.221</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1416</c:v>
+                  <c:v>1417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -957,7 +956,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>(smaller is better, bytes)</a:t>
+              <a:t>(smaller is better, megabytes)</a:t>
             </a:r>
             <a:endParaRPr lang="et-EE"/>
           </a:p>
@@ -1033,10 +1032,10 @@
                 <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>49337312</c:v>
+                  <c:v>49971184</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28491544</c:v>
+                  <c:v>28416552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1165,6 +1164,9 @@
         <c:crossAx val="794333983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1337,10 +1339,10 @@
                 <c:formatCode>_-* #\ ##0_-;\-* #\ ##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>45.728999999999999</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7130000000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4157,7 +4159,7 @@
   <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4190,10 +4192,10 @@
         <v>384</v>
       </c>
       <c r="D3" s="1">
-        <v>3889472</v>
+        <v>5919072</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -4202,15 +4204,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <f>78.468</f>
-        <v>78.468000000000004</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1">
-        <f>1346.181</f>
-        <v>1346.181</v>
+        <v>1323</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -4221,10 +4221,10 @@
         <v>384</v>
       </c>
       <c r="D5" s="1">
-        <v>7522320</v>
+        <v>8682272</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -4232,15 +4232,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <f>208.221</f>
-        <v>208.221</v>
+        <v>188</v>
       </c>
       <c r="D6" s="1">
-        <f>1416</f>
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -4248,10 +4246,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>49337312</v>
+        <v>49971184</v>
       </c>
       <c r="D7" s="1">
-        <v>28491544</v>
+        <v>28416552</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -4262,13 +4260,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>45.728999999999999</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1">
-        <v>2.7130000000000001</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>